<commit_message>
solving name issues_new account
</commit_message>
<xml_diff>
--- a/data/list_meps_2019.xlsx
+++ b/data/list_meps_2019.xlsx
@@ -4656,9 +4656,6 @@
     <t>aliciahoms</t>
   </si>
   <si>
-    <t>IncirEvin</t>
-  </si>
-  <si>
     <t>JackieJonesWal1</t>
   </si>
   <si>
@@ -4885,6 +4882,9 @@
   </si>
   <si>
     <t>isabel_mep</t>
+  </si>
+  <si>
+    <t>EvinIncir</t>
   </si>
 </sst>
 </file>
@@ -5735,8 +5735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E749"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A581" workbookViewId="0">
-      <selection activeCell="B595" sqref="B595"/>
+    <sheetView tabSelected="1" topLeftCell="A311" workbookViewId="0">
+      <selection activeCell="B325" sqref="B325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10946,7 +10946,7 @@
         <v>703</v>
       </c>
       <c r="B316" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="C316" t="s">
         <v>44</v>
@@ -11096,7 +11096,7 @@
         <v>721</v>
       </c>
       <c r="B325" t="s">
-        <v>1545</v>
+        <v>1621</v>
       </c>
       <c r="C325" t="s">
         <v>22</v>
@@ -11260,7 +11260,7 @@
         <v>741</v>
       </c>
       <c r="B335" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="C335" t="s">
         <v>22</v>
@@ -11342,7 +11342,7 @@
         <v>749</v>
       </c>
       <c r="B340" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="C340" t="s">
         <v>6</v>
@@ -11571,10 +11571,10 @@
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A354" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B354" t="s">
         <v>1547</v>
-      </c>
-      <c r="B354" t="s">
-        <v>1548</v>
       </c>
       <c r="C354" t="s">
         <v>27</v>
@@ -11744,7 +11744,7 @@
         <v>801</v>
       </c>
       <c r="B364" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="C364" t="s">
         <v>27</v>
@@ -11809,7 +11809,7 @@
         <v>808</v>
       </c>
       <c r="B368" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="C368" t="s">
         <v>22</v>
@@ -12080,7 +12080,7 @@
         <v>839</v>
       </c>
       <c r="B385" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="C385" t="s">
         <v>27</v>
@@ -12193,7 +12193,7 @@
         <v>850</v>
       </c>
       <c r="B392" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="C392" t="s">
         <v>27</v>
@@ -12210,7 +12210,7 @@
         <v>851</v>
       </c>
       <c r="B393" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="C393" t="s">
         <v>6</v>
@@ -12391,7 +12391,7 @@
         <v>870</v>
       </c>
       <c r="B404" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="C404" t="s">
         <v>18</v>
@@ -12473,7 +12473,7 @@
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A409" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="C409" t="s">
         <v>27</v>
@@ -12490,7 +12490,7 @@
         <v>881</v>
       </c>
       <c r="B410" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="C410" t="s">
         <v>22</v>
@@ -12541,7 +12541,7 @@
         <v>886</v>
       </c>
       <c r="B413" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="C413" t="s">
         <v>22</v>
@@ -12575,7 +12575,7 @@
         <v>889</v>
       </c>
       <c r="B415" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="C415" t="s">
         <v>18</v>
@@ -12705,10 +12705,10 @@
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A423" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B423" t="s">
         <v>1557</v>
-      </c>
-      <c r="B423" t="s">
-        <v>1558</v>
       </c>
       <c r="C423" t="s">
         <v>22</v>
@@ -12793,7 +12793,7 @@
         <v>913</v>
       </c>
       <c r="B428" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="C428" t="s">
         <v>6</v>
@@ -12974,7 +12974,7 @@
         <v>935</v>
       </c>
       <c r="B439" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="C439" t="s">
         <v>6</v>
@@ -13107,7 +13107,7 @@
         <v>950</v>
       </c>
       <c r="B447" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="C447" t="s">
         <v>22</v>
@@ -13175,7 +13175,7 @@
         <v>957</v>
       </c>
       <c r="B451" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="C451" t="s">
         <v>22</v>
@@ -13209,7 +13209,7 @@
         <v>960</v>
       </c>
       <c r="B453" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="C453" t="s">
         <v>22</v>
@@ -13257,10 +13257,10 @@
     </row>
     <row r="456" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A456" t="s">
+        <v>1563</v>
+      </c>
+      <c r="B456" t="s">
         <v>1564</v>
-      </c>
-      <c r="B456" t="s">
-        <v>1565</v>
       </c>
       <c r="C456" t="s">
         <v>18</v>
@@ -13291,7 +13291,7 @@
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A458" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="C458" t="s">
         <v>6</v>
@@ -13370,7 +13370,7 @@
         <v>976</v>
       </c>
       <c r="B463" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="C463" t="s">
         <v>6</v>
@@ -13486,7 +13486,7 @@
         <v>990</v>
       </c>
       <c r="B470" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="C470" t="s">
         <v>6</v>
@@ -13732,7 +13732,7 @@
         <v>1017</v>
       </c>
       <c r="B485" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="C485" t="s">
         <v>6</v>
@@ -13921,10 +13921,10 @@
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
+        <v>1569</v>
+      </c>
+      <c r="B497" t="s">
         <v>1570</v>
-      </c>
-      <c r="B497" t="s">
-        <v>1571</v>
       </c>
       <c r="C497" t="s">
         <v>6</v>
@@ -14139,7 +14139,7 @@
         <v>1062</v>
       </c>
       <c r="B510" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="C510" t="s">
         <v>18</v>
@@ -14408,7 +14408,7 @@
         <v>1094</v>
       </c>
       <c r="B526" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="C526" t="s">
         <v>34</v>
@@ -14524,7 +14524,7 @@
         <v>1106</v>
       </c>
       <c r="B533" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="C533" t="s">
         <v>34</v>
@@ -14725,7 +14725,7 @@
         <v>1130</v>
       </c>
       <c r="B545" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="C545" t="s">
         <v>22</v>
@@ -14759,7 +14759,7 @@
         <v>1133</v>
       </c>
       <c r="B547" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="C547" t="s">
         <v>6</v>
@@ -14776,7 +14776,7 @@
         <v>1135</v>
       </c>
       <c r="B548" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="C548" t="s">
         <v>6</v>
@@ -14807,7 +14807,7 @@
         <v>1138</v>
       </c>
       <c r="B550" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="C550" t="s">
         <v>27</v>
@@ -14841,7 +14841,7 @@
         <v>1141</v>
       </c>
       <c r="B552" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="C552" t="s">
         <v>6</v>
@@ -14875,7 +14875,7 @@
         <v>1144</v>
       </c>
       <c r="B554" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="C554" t="s">
         <v>14</v>
@@ -14991,7 +14991,7 @@
         <v>1156</v>
       </c>
       <c r="B561" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="C561" t="s">
         <v>14</v>
@@ -15144,7 +15144,7 @@
         <v>1175</v>
       </c>
       <c r="B570" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="C570" t="s">
         <v>18</v>
@@ -15246,7 +15246,7 @@
         <v>1187</v>
       </c>
       <c r="B576" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="C576" t="s">
         <v>22</v>
@@ -15331,7 +15331,7 @@
         <v>1196</v>
       </c>
       <c r="B581" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="C581" t="s">
         <v>27</v>
@@ -15348,7 +15348,7 @@
         <v>1197</v>
       </c>
       <c r="B582" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="C582" t="s">
         <v>27</v>
@@ -15478,7 +15478,7 @@
         <v>1212</v>
       </c>
       <c r="B590" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="C590" t="s">
         <v>27</v>
@@ -15563,7 +15563,7 @@
         <v>1221</v>
       </c>
       <c r="B595" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="C595" t="s">
         <v>22</v>
@@ -15679,10 +15679,10 @@
     </row>
     <row r="602" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A602" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="B602" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="C602" t="s">
         <v>22</v>
@@ -15959,7 +15959,7 @@
         <v>1264</v>
       </c>
       <c r="B619" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="C619" t="s">
         <v>6</v>
@@ -16002,10 +16002,10 @@
     </row>
     <row r="622" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A622" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B622" t="s">
         <v>1587</v>
-      </c>
-      <c r="B622" t="s">
-        <v>1588</v>
       </c>
       <c r="C622" t="s">
         <v>6</v>
@@ -16118,7 +16118,7 @@
         <v>1278</v>
       </c>
       <c r="B629" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="C629" t="s">
         <v>6</v>
@@ -16152,7 +16152,7 @@
         <v>1282</v>
       </c>
       <c r="B631" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="C631" t="s">
         <v>44</v>
@@ -16271,7 +16271,7 @@
         <v>1295</v>
       </c>
       <c r="B638" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="C638" t="s">
         <v>6</v>
@@ -16288,7 +16288,7 @@
         <v>1297</v>
       </c>
       <c r="B639" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="C639" t="s">
         <v>44</v>
@@ -16353,10 +16353,10 @@
     </row>
     <row r="643" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A643" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B643" t="s">
         <v>1593</v>
-      </c>
-      <c r="B643" t="s">
-        <v>1594</v>
       </c>
       <c r="C643" t="s">
         <v>6</v>
@@ -16387,7 +16387,7 @@
         <v>1305</v>
       </c>
       <c r="B645" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
       <c r="C645" t="s">
         <v>27</v>
@@ -16786,7 +16786,7 @@
         <v>1353</v>
       </c>
       <c r="B669" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="C669" t="s">
         <v>27</v>
@@ -16851,10 +16851,10 @@
     </row>
     <row r="673" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A673" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B673" t="s">
         <v>1597</v>
-      </c>
-      <c r="B673" t="s">
-        <v>1598</v>
       </c>
       <c r="C673" t="s">
         <v>44</v>
@@ -16888,7 +16888,7 @@
         <v>1363</v>
       </c>
       <c r="B675" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="C675" t="s">
         <v>44</v>
@@ -16987,7 +16987,7 @@
         <v>1376</v>
       </c>
       <c r="B681" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
       <c r="C681" t="s">
         <v>22</v>
@@ -17038,7 +17038,7 @@
         <v>1382</v>
       </c>
       <c r="B684" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
       <c r="C684" t="s">
         <v>6</v>
@@ -17089,7 +17089,7 @@
         <v>1389</v>
       </c>
       <c r="B687" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
       <c r="C687" t="s">
         <v>18</v>
@@ -17106,7 +17106,7 @@
         <v>1390</v>
       </c>
       <c r="B688" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
       <c r="C688" t="s">
         <v>27</v>
@@ -17290,7 +17290,7 @@
         <v>1413</v>
       </c>
       <c r="B699" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="C699" t="s">
         <v>6</v>
@@ -17369,7 +17369,7 @@
         <v>1421</v>
       </c>
       <c r="B704" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
       <c r="C704" t="s">
         <v>34</v>
@@ -17573,7 +17573,7 @@
         <v>1445</v>
       </c>
       <c r="B716" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
       <c r="C716" t="s">
         <v>27</v>
@@ -17641,7 +17641,7 @@
         <v>1453</v>
       </c>
       <c r="B720" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="C720" t="s">
         <v>14</v>
@@ -17765,7 +17765,7 @@
         <v>1464</v>
       </c>
       <c r="B728" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="C728" t="s">
         <v>27</v>
@@ -17915,7 +17915,7 @@
         <v>1480</v>
       </c>
       <c r="B737" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="C737" t="s">
         <v>18</v>
@@ -17963,7 +17963,7 @@
         <v>1484</v>
       </c>
       <c r="B740" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="C740" t="s">
         <v>34</v>
@@ -17980,7 +17980,7 @@
         <v>1486</v>
       </c>
       <c r="B741" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="C741" t="s">
         <v>6</v>
@@ -18028,7 +18028,7 @@
         <v>1490</v>
       </c>
       <c r="B744" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="C744" t="s">
         <v>27</v>
@@ -18079,7 +18079,7 @@
         <v>1495</v>
       </c>
       <c r="B747" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="C747" t="s">
         <v>6</v>

</xml_diff>